<commit_message>
Implement updated post endpoint
</commit_message>
<xml_diff>
--- a/social-media/testcases/Backend.xlsx
+++ b/social-media/testcases/Backend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\7.Golang_WorkSpace\EngineeringPro\BE-K14\social-media\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6371DDCD-DC68-41FC-9E02-0C4474B667FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BAF030-A9C6-4F69-B978-7AED2CA3A041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="170" xr2:uid="{889BDA78-D8A0-4916-8D1E-9392A4CBFB0F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
   <si>
     <t>Endpoints</t>
   </si>
@@ -319,16 +319,6 @@
     <t>content is empty</t>
   </si>
   <si>
-    <t>Should have validate</t>
-  </si>
-  <si>
-    <t>{
-  "errors": {
-    "content": "must be required"
-  }
-}</t>
-  </si>
-  <si>
     <t>{
   "email": "",
   "password": "P@ssword123"
@@ -344,6 +334,109 @@
     <t>{
   "errors": {
     "password": "must be required"
+  }
+}</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Posts</t>
+  </si>
+  <si>
+    <t>{
+  "title": "                 ",
+  "content": "",
+  "userId": 1
+}</t>
+  </si>
+  <si>
+    <t>Blank title or empty content</t>
+  </si>
+  <si>
+    <t>Should be validated</t>
+  </si>
+  <si>
+    <t>{
+  "errors": {
+    "content": "is required",
+    "title": "must be not blank"
+  }
+}</t>
+  </si>
+  <si>
+    <t>get-posts.http</t>
+  </si>
+  <si>
+    <t>GET http://localhost:8080/api/v1/posts</t>
+  </si>
+  <si>
+    <t>Get all posts succesfully</t>
+  </si>
+  <si>
+    <t>{
+  "posts": [
+    {
+      "postId": 9,
+      "title": "Study Golang",
+      "content": "Golang is open source language from Google",
+      "createdAt": "2025-05-04T05:16:01.819Z",
+      "author": {
+        "userId": 6,
+        "firstName": "User 006 Test",
+        "lastName": "Maple Billing Team",
+        "fullName": "User 006 Test Maple Billing Team",
+        "birthday": "1995-05-20T00:00:00Z",
+        "email": "user006@infotrack.com.au",
+        "avatar": null
+      }
+    },
+    {
+      "postId": 8,
+      "title": "Study Golang",
+      "content": "Golang is open source language from Google",
+      "createdAt": "2025-05-04T04:09:12.555Z",
+      "author": {
+        "userId": 6,
+        "firstName": "User 006 Test",
+        "lastName": "Maple Billing Team",
+        "fullName": "User 006 Test Maple Billing Team",
+        "birthday": "1995-05-20T00:00:00Z",
+        "email": "user006@infotrack.com.au",
+        "avatar": null
+      }
+    }]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "errors": {
+    "content": "is required",
+  }
+}</t>
+  </si>
+  <si>
+    <t>GET http://localhost:8080/api/v1/posts/5</t>
+  </si>
+  <si>
+    <t>Get post by id successfully</t>
+  </si>
+  <si>
+    <t>{
+  "post": {
+    "postId": 5,
+    "title": "Deploy Golang App lên Docker",
+    "content": "Việc deploy Golang app vào container rất tiện lợi nhờ Docker.",
+    "createdAt": "2025-05-03T07:56:01.462Z",
+    "author": {
+      "userId": 4,
+      "firstName": "User 004",
+      "lastName": "Global InfoTrack",
+      "fullName": "User 004 - Global InfoTrack",
+      "birthday": "1999-12-24T00:00:00Z",
+      "email": "user004@infotrack.com.au",
+      "avatar": null
+    }
   }
 }</t>
   </si>
@@ -539,6 +632,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -554,17 +656,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -903,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7073E8E9-ACD7-40B7-8508-0731B07445A4}">
-  <dimension ref="A3:I43"/>
+  <dimension ref="A3:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,15 +1016,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="65.400000000000006" x14ac:dyDescent="1.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="A3" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:9" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -963,7 +1058,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -995,27 +1090,27 @@
         <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="21">
+      <c r="F6" s="15">
         <v>400</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
@@ -1040,7 +1135,7 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1055,7 +1150,7 @@
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="14">
         <v>201</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1069,7 +1164,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="8" t="s">
         <v>39</v>
       </c>
@@ -1082,7 +1177,7 @@
       <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="15">
         <v>400</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -1094,13 +1189,13 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
@@ -1119,11 +1214,11 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1142,11 +1237,11 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1214,7 +1309,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>35</v>
       </c>
@@ -1267,15 +1362,17 @@
       <c r="I16" s="2"/>
     </row>
     <row r="31" spans="1:9" ht="65.400000000000006" x14ac:dyDescent="1.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
+      <c r="A31" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
     </row>
     <row r="32" spans="1:9" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
@@ -1306,8 +1403,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="288" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
+    <row r="33" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1322,7 +1419,7 @@
       <c r="E33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="20">
+      <c r="F33" s="14">
         <v>201</v>
       </c>
       <c r="G33" s="6" t="s">
@@ -1333,263 +1430,182 @@
       </c>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
+    <row r="34" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22"/>
       <c r="B34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>57</v>
+      <c r="C34" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="21">
+        <v>66</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="15">
         <v>400</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>13</v>
+    <row r="35" spans="1:9" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="5">
-        <v>201</v>
+        <v>67</v>
+      </c>
+      <c r="F35" s="15">
+        <v>400</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="5">
-        <v>500</v>
+        <v>71</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="14">
+        <v>200</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
-        <v>34</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
       <c r="B37" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="5">
+        <v>74</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="14">
         <v>200</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>22</v>
+      <c r="H37" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="5">
-        <v>401</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="38" spans="1:9" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="3"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
-      <c r="B39" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" s="5">
-        <v>401</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>29</v>
-      </c>
+    <row r="39" spans="1:9" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="19"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="3"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" ht="43.8" x14ac:dyDescent="0.35">
-      <c r="A40" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="2">
-        <v>401</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>29</v>
-      </c>
+    <row r="40" spans="1:9" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="20"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="3"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" ht="43.8" x14ac:dyDescent="0.35">
-      <c r="A41" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>36</v>
-      </c>
+    <row r="41" spans="1:9" ht="36.6" x14ac:dyDescent="0.35">
+      <c r="A41" s="9"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="2">
-        <v>401</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="3"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>36</v>
-      </c>
+    <row r="42" spans="1:9" ht="36.6" x14ac:dyDescent="0.35">
+      <c r="A42" s="9"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F42" s="2">
-        <v>200</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="3"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F43" s="2">
-        <v>200</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>49</v>
-      </c>
+    <row r="43" spans="1:9" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="11"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="4"/>
       <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="11"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A40"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A9"/>

</xml_diff>